<commit_message>
Can load Card data
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Excel/Value/CardValue.xlsx
+++ b/Assets/StreamingAssets/Excel/Value/CardValue.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Downloads\UNR\CS 425\CS425-426\Assets\StreamingAssets\Value\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Downloads\UNR\CS 425\CS425-426\Assets\StreamingAssets\Excel\Value\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDF6C80-5FD5-493F-8485-122D030BEF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44184ED9-9BD2-47F4-BBFE-0C19CABC2E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -78,6 +78,42 @@
   </si>
   <si>
     <t>Rarity (0 = Common, 1 = Rare, 2 =VeryRare, 3 = Epic)</t>
+  </si>
+  <si>
+    <t>Card Type (Weapons)</t>
+  </si>
+  <si>
+    <t>Weapons</t>
+  </si>
+  <si>
+    <t>AK-47</t>
+  </si>
+  <si>
+    <t>Deagle</t>
+  </si>
+  <si>
+    <t>Glock-18</t>
+  </si>
+  <si>
+    <t>HE</t>
+  </si>
+  <si>
+    <t>M4A4</t>
+  </si>
+  <si>
+    <t>PSL</t>
+  </si>
+  <si>
+    <t>Sawed</t>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>UMP</t>
+  </si>
+  <si>
+    <t>UZI</t>
   </si>
 </sst>
 </file>
@@ -395,21 +431,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="4" width="66.109375" customWidth="1"/>
-    <col min="5" max="5" width="74.21875" customWidth="1"/>
+    <col min="2" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="5" max="5" width="66.109375" customWidth="1"/>
+    <col min="6" max="6" width="74.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,16 +453,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>ROW()-2</f>
         <v>0</v>
@@ -434,35 +473,41 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f t="shared" ref="A3:A5" si="0">ROW()-2</f>
+        <f t="shared" ref="A3:A15" si="0">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -470,17 +515,20 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -488,14 +536,227 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added images for the cards
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Excel/Value/CardValue.xlsx
+++ b/Assets/StreamingAssets/Excel/Value/CardValue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Downloads\UNR\CS 425\CS425-426\Assets\StreamingAssets\Excel\Value\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNR Classes\CS 425\Unity Game\CS425-426\Assets\StreamingAssets\Excel\Value\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44184ED9-9BD2-47F4-BBFE-0C19CABC2E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA1DC21-DC43-4CEC-9358-599298C3CB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:F15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Game Menu Interaction Added -- Press X to open and close menu
in the Inventory scene, you can switch between tabs. press X to open and close the menu. The intention is to have the gameMenu object be a prefab you can add to the exploration scenes.

TODO:
Add functionality for all sub-panels:
Implement deck building
  -- allow player to sort cards
Implement Card Combinations
Implement Weapon Upgrades:
Implement options menu buttons
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Excel/Value/CardValue.xlsx
+++ b/Assets/StreamingAssets/Excel/Value/CardValue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNR Classes and Files\CS 425 - Software Engineering\Senior Projects - Game\CS425-426\Assets\StreamingAssets\Excel\Value\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f734f07fa70639b/Documents/GitHub/CS425-426/Assets/StreamingAssets/Excel/Value/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CA5EFD-5273-4130-AB32-818DA4AAA797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F7CA5EFD-5273-4130-AB32-818DA4AAA797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C398C3F-870D-4889-BDB3-9FD9A98C6C4E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1224" yWindow="4308" windowWidth="19404" windowHeight="9372" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,20 +621,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="101.7109375" customWidth="1"/>
-    <col min="7" max="7" width="121.42578125" customWidth="1"/>
+    <col min="2" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="101.6640625" customWidth="1"/>
+    <col min="7" max="7" width="121.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +657,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>ROW()-2</f>
         <v>0</v>
@@ -681,7 +681,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A21" si="0">ROW()-2</f>
         <v>1</v>
@@ -705,7 +705,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -729,7 +729,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -753,7 +753,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -777,7 +777,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -801,7 +801,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -825,7 +825,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -849,7 +849,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -873,7 +873,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -897,7 +897,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -921,7 +921,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -945,7 +945,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -969,7 +969,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -993,7 +993,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1017,7 +1017,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1041,7 +1041,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1065,7 +1065,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1089,7 +1089,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1113,7 +1113,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1137,9 +1137,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f>ROW()-2</f>
+        <f t="shared" ref="A22:A29" si="1">ROW()-2</f>
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -1158,9 +1158,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f>ROW()-2</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -1179,9 +1179,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f>ROW()-2</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -1200,9 +1200,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f>ROW()-2</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -1221,9 +1221,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f>ROW()-2</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -1242,9 +1242,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f>ROW()-2</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -1263,9 +1263,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f>ROW()-2</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -1284,9 +1284,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f>ROW()-2</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B29" t="s">

</xml_diff>